<commit_message>
Don't Pull, test UE not working
</commit_message>
<xml_diff>
--- a/censo/src/main/resources/SitiosEdificioTest.xlsx
+++ b/censo/src/main/resources/SitiosEdificioTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22019"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\RRHH\CENSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="11_6065779BDFD7F06FADE349860CCD4ED9715153E1" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D07B13D9-9262-4727-ABA2-E5CA3DEA3B43}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="11_6065779BDFD7F06FADE349860CCD4ED9715153E1" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{67370D95-88BB-451F-8DAA-80B25DE9DF2F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
   <si>
     <t>IDCOMPLEJO</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>MARTIN</t>
+  </si>
+  <si>
+    <t>0410/1A</t>
   </si>
   <si>
     <t>NUCLEO MÁLAGA</t>
@@ -2535,11 +2538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="D2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2708,10 +2711,10 @@
         <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L4" t="s">
         <v>30</v>
@@ -2722,6 +2725,9 @@
       <c r="R4" t="s">
         <v>32</v>
       </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="K7" s="23"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:XFD1" xr:uid="{EAB1FB10-6EB1-43B4-9923-BFDD9BB2F79C}"/>
@@ -2853,7 +2859,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="B3" s="25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="27"/>
@@ -2973,7 +2979,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F10" s="7">
         <v>4</v>
@@ -2994,7 +3000,7 @@
         <v>9</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O10" s="7">
         <v>10</v>
@@ -3018,7 +3024,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F11" s="7">
         <v>16</v>
@@ -3039,7 +3045,7 @@
         <v>21</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O11" s="7">
         <v>22</v>
@@ -3181,7 +3187,7 @@
         <v>27</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F14" s="7">
         <v>28</v>
@@ -3202,7 +3208,7 @@
         <v>33</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O14" s="7">
         <v>34</v>
@@ -3226,7 +3232,7 @@
         <v>39</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F15" s="7">
         <v>40</v>
@@ -3247,7 +3253,7 @@
         <v>45</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O15" s="7">
         <v>46</v>
@@ -3414,7 +3420,7 @@
         <v>51</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F22" s="24">
         <v>52</v>
@@ -3435,7 +3441,7 @@
         <v>57</v>
       </c>
       <c r="N22" s="24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O22" s="24">
         <v>58</v>
@@ -3458,7 +3464,7 @@
         <v>63</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F23" s="7">
         <v>64</v>
@@ -3479,7 +3485,7 @@
         <v>69</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O23" s="7">
         <v>70</v>
@@ -3618,7 +3624,7 @@
         <v>75</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F26" s="7">
         <v>76</v>
@@ -3639,7 +3645,7 @@
         <v>81</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O26" s="7">
         <v>82</v>
@@ -3662,7 +3668,7 @@
         <v>87</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F27" s="7">
         <v>88</v>
@@ -3683,7 +3689,7 @@
         <v>93</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O27" s="7">
         <v>94</v>
@@ -3847,7 +3853,7 @@
         <v>99</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F33" s="7">
         <v>100</v>
@@ -3868,7 +3874,7 @@
         <v>105</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O33" s="7">
         <v>106</v>
@@ -3891,7 +3897,7 @@
         <v>111</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F34" s="7">
         <v>112</v>
@@ -3912,7 +3918,7 @@
         <v>117</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O34" s="7">
         <v>118</v>
@@ -4051,7 +4057,7 @@
         <v>123</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F37" s="7">
         <v>124</v>
@@ -4072,7 +4078,7 @@
         <v>129</v>
       </c>
       <c r="N37" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="O37" s="7">
         <v>130</v>
@@ -4095,7 +4101,7 @@
         <v>135</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F38" s="7">
         <v>136</v>
@@ -4116,7 +4122,7 @@
         <v>141</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O38" s="7">
         <v>142</v>
@@ -4188,7 +4194,7 @@
     </row>
     <row r="41" spans="2:17">
       <c r="H41" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="2:17" ht="17.25">
@@ -4610,7 +4616,7 @@
     </row>
     <row r="2" spans="1:24">
       <c r="B2" s="25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="27"/>
@@ -4958,7 +4964,7 @@
         <v>179</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R15" s="7">
         <v>180</v>
@@ -5014,7 +5020,7 @@
         <v>196</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R16" s="7">
         <v>197</v>
@@ -5209,7 +5215,7 @@
         <v>210</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M19" s="7">
         <v>211</v>
@@ -5265,7 +5271,7 @@
         <v>227</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M20" s="7">
         <v>228</v>
@@ -5571,7 +5577,7 @@
         <v>244</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L34" s="7">
         <v>245</v>
@@ -5628,7 +5634,7 @@
         <v>261</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L35" s="7">
         <v>262</v>
@@ -5833,7 +5839,7 @@
         <v>278</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L38" s="7">
         <v>279</v>
@@ -5890,7 +5896,7 @@
         <v>295</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L39" s="7">
         <v>296</v>
@@ -6087,7 +6093,7 @@
         <v>306</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L44" s="7">
         <v>307</v>
@@ -6126,7 +6132,7 @@
         <v>317</v>
       </c>
       <c r="K45" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L45" s="7">
         <v>318</v>
@@ -6267,7 +6273,7 @@
         <v>328</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L48" s="7">
         <v>329</v>
@@ -6306,7 +6312,7 @@
         <v>339</v>
       </c>
       <c r="K49" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L49" s="7">
         <v>340</v>
@@ -6494,7 +6500,7 @@
         <v>352</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G55" s="7">
         <v>353</v>
@@ -6551,7 +6557,7 @@
         <v>369</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G56" s="7">
         <v>370</v>
@@ -6758,7 +6764,7 @@
         <v>386</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G59" s="7">
         <v>387</v>
@@ -6815,7 +6821,7 @@
         <v>403</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G60" s="7">
         <v>404</v>
@@ -7509,7 +7515,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -7526,7 +7532,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C2">
         <v>145</v>

</xml_diff>